<commit_message>
Enhanced frame and overlay search with comprehensive diagnostics - added page structure inspection, frame element counting, and element visibility tracking for accurate target detection
</commit_message>
<xml_diff>
--- a/Br.net login .xlsx
+++ b/Br.net login .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\OneDrive\Desktop\Chatgpt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6080D1EA-AC64-4073-9A12-C8D4D83957D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD24A4DE-CBD1-4339-A84A-06AD7F16D725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26A5588D-6DB4-4F1A-9805-B9C41FC223AD}"/>
   </bookViews>
@@ -261,7 +261,7 @@
     <t>Enter User Name</t>
   </si>
   <si>
-    <t>Click To Open</t>
+    <t>Start</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>